<commit_message>
2014 05 26 19:20
Criaçao da tabelas e agenda de atividades
</commit_message>
<xml_diff>
--- a/BD2_2M/T5 - Trigges 2/Agenda de projeto.xlsx
+++ b/BD2_2M/T5 - Trigges 2/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -10,9 +10,9 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$28</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="47">
   <si>
     <t>Ação</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Neimar</t>
   </si>
   <si>
-    <t>Aurélio</t>
-  </si>
-  <si>
     <t>GitHub</t>
   </si>
   <si>
@@ -139,13 +136,76 @@
   </si>
   <si>
     <t>T5 - Trigges 2</t>
+  </si>
+  <si>
+    <t>TAB Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAB Curso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAB Aluno </t>
+  </si>
+  <si>
+    <t>TAB Cidade</t>
+  </si>
+  <si>
+    <t>TAB InscricaoDisciplina</t>
+  </si>
+  <si>
+    <t>TAB Disciplina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAB Livro </t>
+  </si>
+  <si>
+    <t>Aurelio</t>
+  </si>
+  <si>
+    <t>NotPad++</t>
+  </si>
+  <si>
+    <t>Trigeer AtulizaAluno</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>||</t>
+  </si>
+  <si>
+    <t>Questao 1</t>
+  </si>
+  <si>
+    <t>Questao 2</t>
+  </si>
+  <si>
+    <t>Questao 3</t>
+  </si>
+  <si>
+    <t>Questao 4</t>
+  </si>
+  <si>
+    <t>Trigeer ControleRetiradas</t>
+  </si>
+  <si>
+    <t>Trigeer AtulizaInscricao</t>
+  </si>
+  <si>
+    <t>Trigeer ControleMovimentacaRetirada</t>
+  </si>
+  <si>
+    <t>TAB Retiradas</t>
+  </si>
+  <si>
+    <t>neimar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -337,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -405,10 +465,6 @@
     </xf>
     <xf numFmtId="20" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -451,7 +507,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -494,7 +550,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -537,7 +593,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -580,7 +636,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -628,7 +684,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -676,7 +732,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -724,7 +780,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -840,7 +896,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -875,7 +930,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1051,14 +1105,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="17" customWidth="1"/>
     <col min="2" max="2" width="43.140625" style="17" customWidth="1"/>
@@ -1071,27 +1125,27 @@
     <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="15">
+      <c r="A1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="6"/>
       <c r="G1" s="21"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+    <row r="2" spans="1:8" ht="21" customHeight="1">
+      <c r="A2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="22">
         <v>41792</v>
@@ -1099,7 +1153,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="33.75" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1125,15 +1179,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="25.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -1142,22 +1196,22 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="21" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -1166,150 +1220,547 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="C9" s="3"/>
+    <row r="6" spans="1:8" ht="21" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
+    <row r="10" spans="1:8" ht="21" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
+    <row r="11" spans="1:8" ht="21" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="3"/>
+    <row r="12" spans="1:8" ht="21" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="C13" s="25"/>
+    <row r="13" spans="1:8" ht="21" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="3"/>
+    <row r="14" spans="1:8" ht="21" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="21" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>24</v>
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="3">
-        <v>29</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="21" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="3">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="20">
-        <f>COUNTA(B4:B16)</f>
+    <row r="17" spans="1:8" ht="21" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="21" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="21" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="21" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="16">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="21" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="21" customHeight="1">
+      <c r="A22" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="16">
         <v>4</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
+      <c r="E22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="21" customHeight="1">
+      <c r="A23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="16">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="21" customHeight="1">
+      <c r="A24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="21" customHeight="1">
+      <c r="A25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="3">
+        <v>7</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="21" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3">
+        <v>29</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="21" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="3">
+        <v>30</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A28" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="20">
+        <f>COUNTA(B4:B27)</f>
+        <v>24</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G17"/>
+  <autoFilter ref="A3:G28"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>

<commit_message>
2014 06 02 11:01
Criação adas tabs
</commit_message>
<xml_diff>
--- a/BD2_2M/T5 - Trigges 2/Agenda de projeto.xlsx
+++ b/BD2_2M/T5 - Trigges 2/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$28</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -204,8 +204,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -896,6 +896,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -930,6 +931,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1105,14 +1107,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="17" customWidth="1"/>
     <col min="2" max="2" width="43.140625" style="17" customWidth="1"/>
@@ -1125,7 +1128,7 @@
     <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" ht="15">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -1137,7 +1140,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1">
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>22</v>
       </c>
@@ -1153,7 +1156,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="33.75" customHeight="1">
+    <row r="3" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5" customHeight="1">
+    <row r="4" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1203,7 +1206,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1">
+    <row r="5" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1227,7 +1230,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1">
+    <row r="6" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1244,14 +1247,14 @@
         <v>33</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1">
+    <row r="7" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1273,7 +1276,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="21" customHeight="1">
+    <row r="8" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1290,14 +1293,14 @@
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1">
+    <row r="9" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1319,7 +1322,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1">
+    <row r="10" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1336,14 +1339,14 @@
         <v>33</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1">
+    <row r="11" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1365,7 +1368,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1">
+    <row r="12" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1382,14 +1385,14 @@
         <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1">
+    <row r="13" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1414,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="21" customHeight="1">
+    <row r="14" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1428,14 +1431,14 @@
         <v>33</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="21" customHeight="1">
+    <row r="15" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1457,7 +1460,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="21" customHeight="1">
+    <row r="16" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1474,14 +1477,14 @@
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="21" customHeight="1">
+    <row r="17" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1503,7 +1506,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="21" customHeight="1">
+    <row r="18" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1520,14 +1523,14 @@
         <v>33</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="21" customHeight="1">
+    <row r="19" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1552,7 @@
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="21" customHeight="1">
+    <row r="20" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1566,13 +1569,13 @@
         <v>46</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="21" customHeight="1">
+    <row r="21" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="21" customHeight="1">
+    <row r="22" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>8</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="21" customHeight="1">
+    <row r="23" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>8</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="21" customHeight="1">
+    <row r="24" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>8</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="21" customHeight="1">
+    <row r="25" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>8</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="21" customHeight="1">
+    <row r="26" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1720,7 +1723,7 @@
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="21" customHeight="1">
+    <row r="27" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -1744,7 +1747,7 @@
       </c>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1">
+    <row r="28" spans="1:8" s="18" customFormat="1" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>18</v>
       </c>
@@ -1760,7 +1763,19 @@
       <c r="H28" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G28"/>
+  <autoFilter ref="A3:G28">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Criar"/>
+        <filter val="Teste"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="?"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>

<commit_message>
2014 06 03 21:20
Finalização do trabalho trigeer 2
</commit_message>
<xml_diff>
--- a/BD2_2M/T5 - Trigges 2/Agenda de projeto.xlsx
+++ b/BD2_2M/T5 - Trigges 2/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$28</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -204,8 +204,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -896,7 +896,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -931,7 +930,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1107,15 +1105,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="17" customWidth="1"/>
     <col min="2" max="2" width="43.140625" style="17" customWidth="1"/>
@@ -1128,7 +1126,7 @@
     <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="15">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -1140,7 +1138,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="21" customHeight="1">
       <c r="A2" s="27" t="s">
         <v>22</v>
       </c>
@@ -1156,7 +1154,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="33.75" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1182,7 +1180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="25.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1206,7 +1204,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="21" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1230,7 +1228,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="21" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1254,7 +1252,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1276,7 +1274,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="21" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1300,7 +1298,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1322,7 +1320,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="21" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1346,7 +1344,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1368,7 +1366,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="21" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1392,7 +1390,7 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1414,7 +1412,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="21" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1436,7 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1460,7 +1458,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="21" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1484,7 +1482,7 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1506,7 +1504,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="21" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1530,7 +1528,7 @@
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1552,7 +1550,7 @@
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="21" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1575,7 +1573,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1595,7 +1593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="21" customHeight="1">
       <c r="A22" s="17" t="s">
         <v>8</v>
       </c>
@@ -1612,7 +1610,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>34</v>
@@ -1621,7 +1619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="21" customHeight="1">
       <c r="A23" s="17" t="s">
         <v>8</v>
       </c>
@@ -1638,7 +1636,7 @@
         <v>33</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>34</v>
@@ -1647,7 +1645,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="21" customHeight="1">
       <c r="A24" s="17" t="s">
         <v>8</v>
       </c>
@@ -1664,7 +1662,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>34</v>
@@ -1673,7 +1671,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="21" customHeight="1">
       <c r="A25" s="17" t="s">
         <v>8</v>
       </c>
@@ -1690,7 +1688,7 @@
         <v>33</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>34</v>
@@ -1699,7 +1697,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="21" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1716,14 +1714,14 @@
         <v>33</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="21" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -1740,14 +1738,14 @@
         <v>9</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" s="18" customFormat="1" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1">
       <c r="A28" s="11" t="s">
         <v>18</v>
       </c>
@@ -1764,15 +1762,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:G28">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Criar"/>
-        <filter val="Teste"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="0"/>
     <filterColumn colId="5">
-      <filters>
-        <filter val="?"/>
+      <filters blank="1">
+        <filter val="!"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>